<commit_message>
fix mistake on total hours
</commit_message>
<xml_diff>
--- a/Documentation/TimeAccounting_EECS448project.xlsx
+++ b/Documentation/TimeAccounting_EECS448project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\Desktop\eecs448\448_Project_1\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F813B036-CDE7-4BFA-BE5C-C9525891A459}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A71AB7C-E81A-46AF-A3BE-F2ED489721B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10500" yWindow="1177" windowWidth="11625" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10500" yWindow="450" windowWidth="11625" windowHeight="13950" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -454,14 +454,15 @@
     <xf numFmtId="20" fontId="5" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="5" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="46" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="5" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -679,8 +680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="93" zoomScaleNormal="53" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6875" defaultRowHeight="15" customHeight="1"/>
@@ -693,18 +694,18 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="55" t="s">
+      <c r="B1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="56"/>
+      <c r="C1" s="57"/>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2"/>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="56"/>
+      <c r="G1" s="57"/>
       <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
@@ -725,10 +726,10 @@
         <v>8</v>
       </c>
       <c r="Q1" s="8"/>
-      <c r="R1" s="59" t="s">
+      <c r="R1" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="S1" s="61">
+      <c r="S1" s="62">
         <f>R3+R4+R5+R6+R7+R8+R9+R10+R11+R12+R13</f>
         <v>4.4493055555555561</v>
       </c>
@@ -737,16 +738,16 @@
       <c r="A2" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="58"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="59"/>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="59"/>
       <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
@@ -777,8 +778,8 @@
       <c r="Q2" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="60"/>
-      <c r="S2" s="60"/>
+      <c r="R2" s="61"/>
+      <c r="S2" s="63"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
       <c r="A3" s="50">
@@ -1195,7 +1196,7 @@
       <c r="P13" s="22">
         <v>0.64583333333333337</v>
       </c>
-      <c r="Q13" s="62">
+      <c r="Q13" s="55">
         <v>0.8125</v>
       </c>
       <c r="R13" s="47">

</xml_diff>